<commit_message>
changes in about us
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/about_us.xlsx
+++ b/apps/features/backlog/android/about_us.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\features\backlog\android\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\apps\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B82541D-9CFC-48C0-8DDC-491DE00EE56C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D79C2-C54C-4D5C-9D77-5546CF3476D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="39">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -140,6 +140,9 @@
   <si>
     <t>check the design of the subscriptuon code field is as executed or not</t>
   </si>
+  <si>
+    <t>SYMMOBABT-0010</t>
+  </si>
 </sst>
 </file>
 
@@ -193,7 +196,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -293,11 +296,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -335,6 +351,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -819,7 +844,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table_1" displayName="Table_1" ref="A3:G14">
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Test Case ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Prerequisites"/>
@@ -1037,8 +1062,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D11" sqref="D11"/>
+      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1555,14 +1580,18 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="7"/>
-      <c r="B14" s="7"/>
-      <c r="C14" s="7"/>
-      <c r="D14" s="7"/>
-      <c r="E14" s="7"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="7"/>
+    <row r="14" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="17" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="17"/>
+      <c r="C14" s="18"/>
+      <c r="D14" s="17"/>
+      <c r="E14" s="17"/>
+      <c r="F14" s="17" t="s">
+        <v>8</v>
+      </c>
+      <c r="G14" s="19"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
@@ -28916,7 +28945,7 @@
     <mergeCell ref="A1:G2"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F13" xr:uid="{3AC6B797-45EF-4286-8651-EB6F7CC81DC1}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F4:F14" xr:uid="{3AC6B797-45EF-4286-8651-EB6F7CC81DC1}">
       <formula1>"Pass,Fail,N/A"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
add new file in admin panel named add push template
</commit_message>
<xml_diff>
--- a/apps/features/backlog/android/about_us.xlsx
+++ b/apps/features/backlog/android/about_us.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\SymlexVPNTestCases\apps\features\backlog\android\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C3D79C2-C54C-4D5C-9D77-5546CF3476D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B497A3C-0C03-4674-A8D7-79F898311119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -297,23 +297,21 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left/>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -351,13 +349,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -1062,8 +1054,8 @@
   <dimension ref="A1:Z990"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="3" topLeftCell="A10" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E15" sqref="E15"/>
+      <pane ySplit="3" topLeftCell="A12" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1580,18 +1572,18 @@
       <c r="Y13" s="1"/>
       <c r="Z13" s="1"/>
     </row>
-    <row r="14" spans="1:26" ht="48.6" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="17" t="s">
+    <row r="14" spans="1:26" ht="75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B14" s="17"/>
-      <c r="C14" s="18"/>
-      <c r="D14" s="17"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="17" t="s">
+      <c r="B14" s="8"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="19"/>
+      <c r="G14" s="17"/>
       <c r="H14" s="1"/>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>

</xml_diff>